<commit_message>
Corrección de errores de API y consultas a la base de datos
</commit_message>
<xml_diff>
--- a/api/db/scripts/database.xlsx
+++ b/api/db/scripts/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I.Lopez\projects\ScrapActionListAPI\api\db\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DA3295-65D7-4811-8E7A-462CA92223E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B0BBED-9511-4D90-8C7A-6735FFFA0B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{6F522B28-B90A-43D0-83DB-2B4A97FECE3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6F522B28-B90A-43D0-83DB-2B4A97FECE3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Defectives" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="498">
   <si>
     <t>Equipment Adjustment</t>
   </si>
@@ -1513,6 +1513,24 @@
   </si>
   <si>
     <t>Subquery</t>
+  </si>
+  <si>
+    <t>FTE</t>
+  </si>
+  <si>
+    <t>FTE Automotive</t>
+  </si>
+  <si>
+    <t>IMT</t>
+  </si>
+  <si>
+    <t>IMTEC</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>Daystar</t>
   </si>
 </sst>
 </file>
@@ -2190,16 +2208,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9954483C-2846-40F9-8B36-E2512D2C7F17}">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="96" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2548,6 +2566,42 @@
       <c r="D30" t="str">
         <f>"INSERT INTO client(id, name) VALUES ('" &amp; B30 &amp; "', '" &amp; C30 &amp; "');"</f>
         <v>INSERT INTO client(id, name) VALUES ('XXX', 'Defaut');</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="D31" t="str">
+        <f>"INSERT INTO client(id, name) VALUES ('" &amp; B31 &amp; "', '" &amp; C31 &amp; "');"</f>
+        <v>INSERT INTO client(id, name) VALUES ('FTE', 'FTE Automotive');</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="D32" t="str">
+        <f>"INSERT INTO client(id, name) VALUES ('" &amp; B32 &amp; "', '" &amp; C32 &amp; "');"</f>
+        <v>INSERT INTO client(id, name) VALUES ('IMT', 'IMTEC');</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="D33" t="str">
+        <f>"INSERT INTO client(id, name) VALUES ('" &amp; B33 &amp; "', '" &amp; C33 &amp; "');"</f>
+        <v>INSERT INTO client(id, name) VALUES ('DAY', 'Daystar');</v>
       </c>
     </row>
   </sheetData>
@@ -2767,8 +2821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C142A0C3-09E0-48C4-88AE-3A11D62508CB}">
   <dimension ref="B2:I489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H489" sqref="H2:H489"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16248,7 +16302,7 @@
         <v>236</v>
       </c>
       <c r="C451" s="9" t="str">
-        <f t="shared" ref="C451:C514" si="28">UPPER(B451)</f>
+        <f t="shared" ref="C451:C489" si="28">UPPER(B451)</f>
         <v>VAL-7121-302</v>
       </c>
       <c r="D451" s="10" t="s">

</xml_diff>

<commit_message>
Inicio de controlador para crear y ajuste de base de datos
</commit_message>
<xml_diff>
--- a/api/db/scripts/database.xlsx
+++ b/api/db/scripts/database.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I.Lopez\projects\ScrapActionListAPI\api\db\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B0BBED-9511-4D90-8C7A-6735FFFA0B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DE19A7-ABAD-40F2-B454-53A2D74CA7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6F522B28-B90A-43D0-83DB-2B4A97FECE3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{6F522B28-B90A-43D0-83DB-2B4A97FECE3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Defectives" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
     <sheet name="Missing client" sheetId="4" r:id="rId3"/>
     <sheet name="Parts" sheetId="3" r:id="rId4"/>
+    <sheet name="Departments" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="515">
   <si>
     <t>Equipment Adjustment</t>
   </si>
@@ -1531,6 +1532,57 @@
   </si>
   <si>
     <t>Daystar</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>r.gomez</t>
+  </si>
+  <si>
+    <t>mario.sanchez</t>
+  </si>
+  <si>
+    <t>Auomation</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Abiu</t>
+  </si>
+  <si>
+    <t>maintenance</t>
+  </si>
+  <si>
+    <t>jorge torres</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Fco. Martinez</t>
+  </si>
+  <si>
+    <t>Supply chain</t>
+  </si>
+  <si>
+    <t>Juan Zuñiga</t>
+  </si>
+  <si>
+    <t>Human Resources</t>
+  </si>
+  <si>
+    <t>Ana Garcia</t>
   </si>
 </sst>
 </file>
@@ -2210,7 +2262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9954483C-2846-40F9-8B36-E2512D2C7F17}">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2614,7 +2666,7 @@
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17476,4 +17528,131 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1089E27A-F4F1-48B7-B635-4CF611449BF0}">
+  <dimension ref="B2:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="75.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>500</v>
+      </c>
+      <c r="C3" t="s">
+        <v>501</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"INSERT INTO department(name, manager) VALUES ('"&amp;B3&amp;"', '"&amp;C3&amp;"');"</f>
+        <v>INSERT INTO department(name, manager) VALUES ('Quality', 'r.gomez');</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>502</v>
+      </c>
+      <c r="D4" t="str">
+        <f>"INSERT INTO department(name, manager) VALUES ('"&amp;B4&amp;"', '"&amp;C4&amp;"');"</f>
+        <v>INSERT INTO department(name, manager) VALUES ('NPI', 'mario.sanchez');</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>503</v>
+      </c>
+      <c r="C5" t="s">
+        <v>504</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" ref="D5:D9" si="0">"INSERT INTO department(name, manager) VALUES ('"&amp;B5&amp;"', '"&amp;C5&amp;"');"</f>
+        <v>INSERT INTO department(name, manager) VALUES ('Auomation', 'set');</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>505</v>
+      </c>
+      <c r="C6" t="s">
+        <v>506</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO department(name, manager) VALUES ('Engineering', 'Abiu');</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>507</v>
+      </c>
+      <c r="C7" t="s">
+        <v>508</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO department(name, manager) VALUES ('maintenance', 'jorge torres');</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>509</v>
+      </c>
+      <c r="C8" t="s">
+        <v>510</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO department(name, manager) VALUES ('Manufacturing', 'Fco. Martinez');</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>511</v>
+      </c>
+      <c r="C9" t="s">
+        <v>512</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO department(name, manager) VALUES ('Supply chain', 'Juan Zuñiga');</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>513</v>
+      </c>
+      <c r="C10" t="s">
+        <v>514</v>
+      </c>
+      <c r="D10" t="str">
+        <f>"INSERT INTO department(name, manager) VALUES ('"&amp;B10&amp;"', '"&amp;C10&amp;"');"</f>
+        <v>INSERT INTO department(name, manager) VALUES ('Human Resources', 'Ana Garcia');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Arreglo de base de datos y crear nuevo issue
</commit_message>
<xml_diff>
--- a/api/db/scripts/database.xlsx
+++ b/api/db/scripts/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I.Lopez\projects\ScrapActionListAPI\api\db\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DE19A7-ABAD-40F2-B454-53A2D74CA7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED82A83-21ED-4C2E-A13E-79003993ABBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{6F522B28-B90A-43D0-83DB-2B4A97FECE3C}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{6F522B28-B90A-43D0-83DB-2B4A97FECE3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Defectives" sheetId="1" r:id="rId1"/>
@@ -1552,37 +1552,37 @@
     <t>Auomation</t>
   </si>
   <si>
-    <t>set</t>
-  </si>
-  <si>
     <t>Engineering</t>
   </si>
   <si>
-    <t>Abiu</t>
-  </si>
-  <si>
     <t>maintenance</t>
   </si>
   <si>
-    <t>jorge torres</t>
-  </si>
-  <si>
     <t>Manufacturing</t>
   </si>
   <si>
-    <t>Fco. Martinez</t>
-  </si>
-  <si>
     <t>Supply chain</t>
   </si>
   <si>
-    <t>Juan Zuñiga</t>
-  </si>
-  <si>
     <t>Human Resources</t>
   </si>
   <si>
-    <t>Ana Garcia</t>
+    <t>Set.Guzman</t>
+  </si>
+  <si>
+    <t>Abiu.Esparza</t>
+  </si>
+  <si>
+    <t>jorge.torres</t>
+  </si>
+  <si>
+    <t>Francisco.Martinez</t>
+  </si>
+  <si>
+    <t>juan.zuniga</t>
+  </si>
+  <si>
+    <t>Ana.Garcia</t>
   </si>
 </sst>
 </file>
@@ -17535,7 +17535,7 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D5" sqref="D5:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17585,71 +17585,71 @@
         <v>503</v>
       </c>
       <c r="C5" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D9" si="0">"INSERT INTO department(name, manager) VALUES ('"&amp;B5&amp;"', '"&amp;C5&amp;"');"</f>
-        <v>INSERT INTO department(name, manager) VALUES ('Auomation', 'set');</v>
+        <v>INSERT INTO department(name, manager) VALUES ('Auomation', 'Set.Guzman');</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C6" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO department(name, manager) VALUES ('Engineering', 'Abiu');</v>
+        <v>INSERT INTO department(name, manager) VALUES ('Engineering', 'Abiu.Esparza');</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C7" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO department(name, manager) VALUES ('maintenance', 'jorge torres');</v>
+        <v>INSERT INTO department(name, manager) VALUES ('maintenance', 'jorge.torres');</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C8" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO department(name, manager) VALUES ('Manufacturing', 'Fco. Martinez');</v>
+        <v>INSERT INTO department(name, manager) VALUES ('Manufacturing', 'Francisco.Martinez');</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C9" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO department(name, manager) VALUES ('Supply chain', 'Juan Zuñiga');</v>
+        <v>INSERT INTO department(name, manager) VALUES ('Supply chain', 'juan.zuniga');</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C10" t="s">
         <v>514</v>
       </c>
       <c r="D10" t="str">
         <f>"INSERT INTO department(name, manager) VALUES ('"&amp;B10&amp;"', '"&amp;C10&amp;"');"</f>
-        <v>INSERT INTO department(name, manager) VALUES ('Human Resources', 'Ana Garcia');</v>
+        <v>INSERT INTO department(name, manager) VALUES ('Human Resources', 'Ana.Garcia');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cerrar issue y actualizado de db
</commit_message>
<xml_diff>
--- a/api/db/scripts/database.xlsx
+++ b/api/db/scripts/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I.Lopez\projects\ScrapActionListAPI\api\db\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED82A83-21ED-4C2E-A13E-79003993ABBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C541E2-67BE-4311-AE3C-B108A37854CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{6F522B28-B90A-43D0-83DB-2B4A97FECE3C}"/>
   </bookViews>
@@ -1549,15 +1549,9 @@
     <t>mario.sanchez</t>
   </si>
   <si>
-    <t>Auomation</t>
-  </si>
-  <si>
     <t>Engineering</t>
   </si>
   <si>
-    <t>maintenance</t>
-  </si>
-  <si>
     <t>Manufacturing</t>
   </si>
   <si>
@@ -1583,6 +1577,12 @@
   </si>
   <si>
     <t>Ana.Garcia</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Automation</t>
   </si>
 </sst>
 </file>
@@ -17535,7 +17535,7 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D10"/>
+      <selection activeCell="D3" sqref="D3:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17582,22 +17582,22 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>503</v>
+        <v>514</v>
       </c>
       <c r="C5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D9" si="0">"INSERT INTO department(name, manager) VALUES ('"&amp;B5&amp;"', '"&amp;C5&amp;"');"</f>
-        <v>INSERT INTO department(name, manager) VALUES ('Auomation', 'Set.Guzman');</v>
+        <v>INSERT INTO department(name, manager) VALUES ('Automation', 'Set.Guzman');</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C6" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -17606,22 +17606,22 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="C7" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO department(name, manager) VALUES ('maintenance', 'jorge.torres');</v>
+        <v>INSERT INTO department(name, manager) VALUES ('Maintenance', 'jorge.torres');</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C8" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -17630,10 +17630,10 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C9" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -17642,10 +17642,10 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C10" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D10" t="str">
         <f>"INSERT INTO department(name, manager) VALUES ('"&amp;B10&amp;"', '"&amp;C10&amp;"');"</f>

</xml_diff>